<commit_message>
Enhance Kordiam example script with more detailed sample data and columns
Co-authored-by: nielsulrik.zepp <nielsulrik.zepp@gmail.com>
</commit_message>
<xml_diff>
--- a/kordiam_example.xlsx
+++ b/kordiam_example.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,31 +437,44 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="1" max="1"/>
     <col width="29" customWidth="1" min="2" max="2"/>
-    <col width="36" customWidth="1" min="3" max="3"/>
+    <col width="40" customWidth="1" min="3" max="3"/>
     <col width="16" customWidth="1" min="4" max="4"/>
     <col width="16" customWidth="1" min="5" max="5"/>
     <col width="16" customWidth="1" min="6" max="6"/>
     <col width="18" customWidth="1" min="7" max="7"/>
     <col width="21" customWidth="1" min="8" max="8"/>
     <col width="21" customWidth="1" min="9" max="9"/>
-    <col width="39" customWidth="1" min="10" max="10"/>
-    <col width="30" customWidth="1" min="11" max="11"/>
-    <col width="23" customWidth="1" min="12" max="12"/>
-    <col width="13" customWidth="1" min="13" max="13"/>
-    <col width="13" customWidth="1" min="14" max="14"/>
-    <col width="9" customWidth="1" min="15" max="15"/>
+    <col width="42" customWidth="1" min="10" max="10"/>
+    <col width="26" customWidth="1" min="11" max="11"/>
+    <col width="36" customWidth="1" min="12" max="12"/>
+    <col width="41" customWidth="1" min="13" max="13"/>
+    <col width="23" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
     <col width="13" customWidth="1" min="16" max="16"/>
-    <col width="21" customWidth="1" min="17" max="17"/>
-    <col width="18" customWidth="1" min="18" max="18"/>
-    <col width="8" customWidth="1" min="19" max="19"/>
-    <col width="7" customWidth="1" min="20" max="20"/>
-    <col width="17" customWidth="1" min="21" max="21"/>
-    <col width="13" customWidth="1" min="22" max="22"/>
-    <col width="9" customWidth="1" min="23" max="23"/>
-    <col width="21" customWidth="1" min="24" max="24"/>
+    <col width="9" customWidth="1" min="17" max="17"/>
+    <col width="13" customWidth="1" min="18" max="18"/>
+    <col width="21" customWidth="1" min="19" max="19"/>
+    <col width="18" customWidth="1" min="20" max="20"/>
+    <col width="8" customWidth="1" min="21" max="21"/>
+    <col width="43" customWidth="1" min="22" max="22"/>
+    <col width="25" customWidth="1" min="23" max="23"/>
+    <col width="39" customWidth="1" min="24" max="24"/>
     <col width="21" customWidth="1" min="25" max="25"/>
+    <col width="7" customWidth="1" min="26" max="26"/>
+    <col width="11" customWidth="1" min="27" max="27"/>
+    <col width="31" customWidth="1" min="28" max="28"/>
+    <col width="20" customWidth="1" min="29" max="29"/>
+    <col width="13" customWidth="1" min="30" max="30"/>
+    <col width="9" customWidth="1" min="31" max="31"/>
+    <col width="34" customWidth="1" min="32" max="32"/>
+    <col width="13" customWidth="1" min="33" max="33"/>
+    <col width="12" customWidth="1" min="34" max="34"/>
+    <col width="21" customWidth="1" min="35" max="35"/>
+    <col width="21" customWidth="1" min="36" max="36"/>
+    <col width="21" customWidth="1" min="37" max="37"/>
+    <col width="21" customWidth="1" min="38" max="38"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -517,84 +530,149 @@
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
+          <t>External Link Title</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Custom Upload Link</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
           <t>Task Note</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Publication Status ID</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Platform ID</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Category ID</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Type ID</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>External ID</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Publication Date</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Task Assignments</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>CMS ID</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Published Content URL</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Published Content Title</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>CMS Edit URL</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>CMS Edit Title</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>Scope</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>Group IDs</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Location Name</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>Street</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>Postal Code</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>Directions</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>City</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>Country</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>State Code</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
         <is>
           <t>Event Start Date</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>Event Start Time</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
         <is>
           <t>Event End Date</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>Event End Time</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Breaking: Local Election Results</t>
+          <t>Breaking: Local Election Results Announced</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -604,7 +682,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Priority story for front page</t>
+          <t>Priority story for front page coverage</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -632,68 +710,129 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Interview the mayor</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
+          <t>Election Coverage System</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>http://upload.example.com/election</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>Interview the mayor and key candidates</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
         <v>3</v>
       </c>
-      <c r="M2" t="n">
+      <c r="O2" t="n">
         <v>1</v>
       </c>
-      <c r="N2" t="n">
+      <c r="P2" t="n">
         <v>8</v>
       </c>
-      <c r="O2" t="n">
+      <c r="Q2" t="n">
         <v>4</v>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="R2" t="inlineStr">
         <is>
           <t>ext_001</t>
         </is>
       </c>
-      <c r="Q2" s="2" t="n">
+      <c r="S2" s="2" t="n">
         <v>45366.75</v>
       </c>
-      <c r="R2" t="inlineStr">
+      <c r="T2" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="S2" t="inlineStr">
+      <c r="U2" t="inlineStr">
         <is>
           <t>667</t>
         </is>
       </c>
-      <c r="T2" t="n">
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>https://news.example.com/election-results</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>Election Results Live</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>https://cms.example.com/edit/election</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>Edit Election Story</t>
+        </is>
+      </c>
+      <c r="Z2" t="n">
         <v>12.5</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>City Hall</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>5,8</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>City Hall Main Auditorium</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>123 Main Street</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>12345</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>Enter through main entrance</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
         <is>
           <t>Springfield</t>
         </is>
       </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="X2" s="2" t="n">
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="AI2" s="2" t="n">
         <v>45366.79166666666</v>
       </c>
-      <c r="Y2" s="2" t="n">
+      <c r="AJ2" s="2" t="n">
+        <v>45366.79166666666</v>
+      </c>
+      <c r="AK2" s="2" t="n">
+        <v>45366.875</v>
+      </c>
+      <c r="AL2" s="2" t="n">
         <v>45366.875</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Weather Update: Storm Warning</t>
+          <t>Weather Alert: Severe Storm Warning</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -731,256 +870,587 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Get meteorologist quote</t>
-        </is>
-      </c>
-      <c r="L3" t="n">
+          <t>Weather Alert Portal</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>http://upload.example.com/weather</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>Get meteorologist quote and safety tips</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
         <v>3</v>
       </c>
-      <c r="M3" t="n">
+      <c r="O3" t="n">
         <v>2</v>
       </c>
-      <c r="N3" t="n">
+      <c r="P3" t="n">
         <v>12</v>
       </c>
-      <c r="O3" t="n">
+      <c r="Q3" t="n">
         <v>5</v>
       </c>
-      <c r="P3" t="inlineStr">
+      <c r="R3" t="inlineStr">
         <is>
           <t>ext_002</t>
         </is>
       </c>
-      <c r="Q3" s="2" t="n">
+      <c r="S3" s="2" t="n">
         <v>45366.25</v>
       </c>
-      <c r="R3" t="inlineStr">
+      <c r="T3" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="U3" t="inlineStr">
         <is>
           <t>668</t>
         </is>
       </c>
-      <c r="T3" t="n">
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>https://news.example.com/storm-warning</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>Storm Warning Alert</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>https://cms.example.com/edit/weather</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>Edit Weather Alert</t>
+        </is>
+      </c>
+      <c r="Z3" t="n">
         <v>8</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>Weather Station</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>Downtown Weather Station</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>456 Weather Ave</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>54321</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>Use north parking lot</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>Springfield</t>
         </is>
       </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sports: Championship Game Tonight</t>
+          <t>Community Event: Annual Festival Planning</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>championship-game-tonight</t>
+          <t>annual-festival-planning</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Get photos from the game</t>
+          <t>Coordinate with events team</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>2</v>
       </c>
       <c r="F4" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G4" t="n">
         <v>7</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>45366.91666666666</v>
+        <v>45383.5</v>
       </c>
       <c r="I4" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>http://sports.example.com/game/456</t>
+          <t>http://events.example.com/festival/2024</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Stadium access arranged</t>
-        </is>
-      </c>
-      <c r="L4" t="n">
+          <t>Event Management</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Coordinate with festival organizers</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>2</v>
       </c>
-      <c r="M4" t="n">
+      <c r="O4" t="n">
         <v>1</v>
       </c>
-      <c r="N4" t="n">
-        <v>15</v>
-      </c>
-      <c r="O4" t="n">
-        <v>4</v>
-      </c>
-      <c r="P4" t="inlineStr">
+      <c r="P4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>6</v>
+      </c>
+      <c r="R4" t="inlineStr">
         <is>
           <t>ext_003</t>
         </is>
       </c>
-      <c r="Q4" s="2" t="n">
-        <v>45367</v>
-      </c>
-      <c r="R4" t="inlineStr">
+      <c r="S4" s="2" t="n">
+        <v>45383.41666666666</v>
+      </c>
+      <c r="T4" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="U4" t="inlineStr">
         <is>
           <t>669</t>
         </is>
       </c>
-      <c r="T4" t="n">
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>https://news.example.com/festival-2024</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>Festival 2024 Preview</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>https://cms.example.com/edit/festival</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>Edit Festival Story</t>
+        </is>
+      </c>
+      <c r="Z4" t="n">
         <v>15.2</v>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>Sports Arena</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>5,8,15</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>Central Park Festival Grounds</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>789 Park Boulevard</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>67890</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>Festival entrance on east side</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>Springfield</t>
         </is>
       </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="X4" s="2" t="n">
-        <v>45366.8125</v>
-      </c>
-      <c r="Y4" s="2" t="n">
-        <v>45366.91666666666</v>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="AI4" s="2" t="n">
+        <v>45383.375</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>45383.375</v>
+      </c>
+      <c r="AK4" s="2" t="n">
+        <v>45383.75</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>45383.75</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Community Event: Farmers Market</t>
+          <t>Sports Update: Championship Game Preview</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>farmers-market-saturday</t>
+          <t>championship-game-preview</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Include vendor list</t>
+          <t>Interview team coaches</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G5" t="n">
         <v>5</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>45367.41666666666</v>
+        <v>45371.75</v>
       </c>
       <c r="I5" t="n">
         <v>-2</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>http://events.example.com/market/789</t>
+          <t>http://sports.example.com/championship</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Confirm vendor participation</t>
-        </is>
-      </c>
-      <c r="L5" t="n">
+          <t>Sports Coverage Hub</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>http://upload.example.com/sports</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Schedule interviews with team coaches</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>3</v>
+      </c>
+      <c r="O5" t="n">
+        <v>3</v>
+      </c>
+      <c r="P5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>ext_004</t>
+        </is>
+      </c>
+      <c r="S5" s="2" t="n">
+        <v>45371.83333333334</v>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>670</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>https://sports.example.com/championship</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Championship Coverage</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>https://cms.example.com/edit/sports</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Edit Sports Story</t>
+        </is>
+      </c>
+      <c r="Z5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>Sports Complex Arena</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>321 Sports Drive</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>98765</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>Use main arena entrance</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>Springfield</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="AI5" s="2" t="n">
+        <v>45371.8125</v>
+      </c>
+      <c r="AJ5" s="2" t="n">
+        <v>45371.8125</v>
+      </c>
+      <c r="AK5" s="2" t="n">
+        <v>45371.91666666666</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <v>45371.91666666666</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Health News: New Medical Center Opens</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>new-medical-center-opens</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Get quotes from medical staff</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" t="n">
+        <v>21</v>
+      </c>
+      <c r="G6" t="n">
+        <v>9</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>45376.60416666666</v>
+      </c>
+      <c r="I6" t="n">
         <v>1</v>
       </c>
-      <c r="M5" t="n">
-        <v>3</v>
-      </c>
-      <c r="N5" t="n">
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>http://health.example.com/medical-center</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Health News Portal</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>Tour new facilities and interview staff</t>
+        </is>
+      </c>
+      <c r="N6" t="n">
+        <v>1</v>
+      </c>
+      <c r="O6" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" t="n">
         <v>10</v>
       </c>
-      <c r="O5" t="n">
-        <v>6</v>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>ext_004</t>
-        </is>
-      </c>
-      <c r="Q5" s="2" t="n">
-        <v>45367.33333333334</v>
-      </c>
-      <c r="R5" t="inlineStr">
+      <c r="Q6" t="n">
+        <v>7</v>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>ext_005</t>
+        </is>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>45376.66666666666</v>
+      </c>
+      <c r="T6" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>670</t>
-        </is>
-      </c>
-      <c r="T5" t="n">
-        <v>5</v>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>Town Square</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>671</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>https://health.example.com/medical-center</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>Medical Center Opening</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>https://cms.example.com/edit/health</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>Edit Health Story</t>
+        </is>
+      </c>
+      <c r="Z6" t="n">
+        <v>11.8</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>8,12</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>New Medical Center Building</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>654 Health Street</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>13579</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>Patient entrance on ground floor</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
         <is>
           <t>Springfield</t>
         </is>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>US</t>
-        </is>
-      </c>
-      <c r="X5" s="2" t="n">
-        <v>45367.375</v>
-      </c>
-      <c r="Y5" s="2" t="n">
-        <v>45367.58333333334</v>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>IL</t>
+        </is>
+      </c>
+      <c r="AI6" s="2" t="n">
+        <v>45376.41666666666</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>45376.41666666666</v>
+      </c>
+      <c r="AK6" s="2" t="n">
+        <v>45376.5</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>45376.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>